<commit_message>
sync on Wed 07/23/2025  1:00:58.66
</commit_message>
<xml_diff>
--- a/option_rank.xlsx
+++ b/option_rank.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K110"/>
+  <dimension ref="A1:K221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5201,6 +5201,4717 @@
         </is>
       </c>
     </row>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G113" t="n">
+        <v>170</v>
+      </c>
+      <c r="H113" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I113" t="n">
+        <v>212552</v>
+      </c>
+      <c r="J113" t="n">
+        <v>0</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G114" t="n">
+        <v>165</v>
+      </c>
+      <c r="H114" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I114" t="n">
+        <v>144952</v>
+      </c>
+      <c r="J114" t="n">
+        <v>0</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G115" t="n">
+        <v>167.5</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="I115" t="n">
+        <v>139000</v>
+      </c>
+      <c r="J115" t="n">
+        <v>0</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G116" t="n">
+        <v>172.5</v>
+      </c>
+      <c r="H116" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I116" t="n">
+        <v>129616</v>
+      </c>
+      <c r="J116" t="n">
+        <v>0</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G117" t="n">
+        <v>167.5</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0</v>
+      </c>
+      <c r="I117" t="n">
+        <v>105853</v>
+      </c>
+      <c r="J117" t="n">
+        <v>0</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G118" t="n">
+        <v>175</v>
+      </c>
+      <c r="H118" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I118" t="n">
+        <v>100403</v>
+      </c>
+      <c r="J118" t="n">
+        <v>0</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G119" t="n">
+        <v>160</v>
+      </c>
+      <c r="H119" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I119" t="n">
+        <v>59623</v>
+      </c>
+      <c r="J119" t="n">
+        <v>0</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G120" t="n">
+        <v>165</v>
+      </c>
+      <c r="H120" t="n">
+        <v>0</v>
+      </c>
+      <c r="I120" t="n">
+        <v>59431</v>
+      </c>
+      <c r="J120" t="n">
+        <v>0</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G121" t="n">
+        <v>180</v>
+      </c>
+      <c r="H121" t="n">
+        <v>25</v>
+      </c>
+      <c r="I121" t="n">
+        <v>59339</v>
+      </c>
+      <c r="J121" t="n">
+        <v>0</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Nvidia</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>167.03</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G122" t="n">
+        <v>162.5</v>
+      </c>
+      <c r="H122" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I122" t="n">
+        <v>48952</v>
+      </c>
+      <c r="J122" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="123"/>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G124" t="n">
+        <v>330</v>
+      </c>
+      <c r="H124" t="n">
+        <v>0</v>
+      </c>
+      <c r="I124" t="n">
+        <v>49752</v>
+      </c>
+      <c r="J124" t="n">
+        <v>0</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G125" t="n">
+        <v>330</v>
+      </c>
+      <c r="H125" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="I125" t="n">
+        <v>45412</v>
+      </c>
+      <c r="J125" t="n">
+        <v>0</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G126" t="n">
+        <v>335</v>
+      </c>
+      <c r="H126" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I126" t="n">
+        <v>29481</v>
+      </c>
+      <c r="J126" t="n">
+        <v>0</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G127" t="n">
+        <v>300</v>
+      </c>
+      <c r="H127" t="n">
+        <v>25</v>
+      </c>
+      <c r="I127" t="n">
+        <v>27554</v>
+      </c>
+      <c r="J127" t="n">
+        <v>0</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G128" t="n">
+        <v>350</v>
+      </c>
+      <c r="H128" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I128" t="n">
+        <v>26951</v>
+      </c>
+      <c r="J128" t="n">
+        <v>0</v>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G129" t="n">
+        <v>340</v>
+      </c>
+      <c r="H129" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I129" t="n">
+        <v>24484</v>
+      </c>
+      <c r="J129" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G130" t="n">
+        <v>325</v>
+      </c>
+      <c r="H130" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I130" t="n">
+        <v>24404</v>
+      </c>
+      <c r="J130" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G131" t="n">
+        <v>310</v>
+      </c>
+      <c r="H131" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I131" t="n">
+        <v>22951</v>
+      </c>
+      <c r="J131" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G132" t="n">
+        <v>320</v>
+      </c>
+      <c r="H132" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I132" t="n">
+        <v>19354</v>
+      </c>
+      <c r="J132" t="n">
+        <v>0</v>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>332.11</v>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G133" t="n">
+        <v>332.5</v>
+      </c>
+      <c r="H133" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="I133" t="n">
+        <v>19201</v>
+      </c>
+      <c r="J133" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="134"/>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G135" t="n">
+        <v>215</v>
+      </c>
+      <c r="H135" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="I135" t="n">
+        <v>149697</v>
+      </c>
+      <c r="J135" t="n">
+        <v>0</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G136" t="n">
+        <v>212.5</v>
+      </c>
+      <c r="H136" t="n">
+        <v>0</v>
+      </c>
+      <c r="I136" t="n">
+        <v>66684</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G137" t="n">
+        <v>220</v>
+      </c>
+      <c r="H137" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I137" t="n">
+        <v>55371</v>
+      </c>
+      <c r="J137" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G138" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="H138" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I138" t="n">
+        <v>53033</v>
+      </c>
+      <c r="J138" t="n">
+        <v>0</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G139" t="n">
+        <v>212.5</v>
+      </c>
+      <c r="H139" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I139" t="n">
+        <v>36396</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G140" t="n">
+        <v>210</v>
+      </c>
+      <c r="H140" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I140" t="n">
+        <v>23081</v>
+      </c>
+      <c r="J140" t="n">
+        <v>0</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G141" t="n">
+        <v>225</v>
+      </c>
+      <c r="H141" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I141" t="n">
+        <v>14086</v>
+      </c>
+      <c r="J141" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G142" t="n">
+        <v>220</v>
+      </c>
+      <c r="H142" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I142" t="n">
+        <v>12999</v>
+      </c>
+      <c r="J142" t="n">
+        <v>0</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G143" t="n">
+        <v>215</v>
+      </c>
+      <c r="H143" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="I143" t="n">
+        <v>12342</v>
+      </c>
+      <c r="J143" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>214.4</v>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G144" t="n">
+        <v>215</v>
+      </c>
+      <c r="H144" t="n">
+        <v>0</v>
+      </c>
+      <c r="I144" t="n">
+        <v>11497</v>
+      </c>
+      <c r="J144" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="145"/>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G146" t="n">
+        <v>155</v>
+      </c>
+      <c r="H146" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="I146" t="n">
+        <v>54637</v>
+      </c>
+      <c r="J146" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G147" t="n">
+        <v>160</v>
+      </c>
+      <c r="H147" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I147" t="n">
+        <v>48796</v>
+      </c>
+      <c r="J147" t="n">
+        <v>0</v>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G148" t="n">
+        <v>150</v>
+      </c>
+      <c r="H148" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I148" t="n">
+        <v>44249</v>
+      </c>
+      <c r="J148" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G149" t="n">
+        <v>157.5</v>
+      </c>
+      <c r="H149" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I149" t="n">
+        <v>31577</v>
+      </c>
+      <c r="J149" t="n">
+        <v>0</v>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G150" t="n">
+        <v>152.5</v>
+      </c>
+      <c r="H150" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I150" t="n">
+        <v>26537</v>
+      </c>
+      <c r="J150" t="n">
+        <v>0</v>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G151" t="n">
+        <v>152.5</v>
+      </c>
+      <c r="H151" t="n">
+        <v>0</v>
+      </c>
+      <c r="I151" t="n">
+        <v>23070</v>
+      </c>
+      <c r="J151" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G152" t="n">
+        <v>165</v>
+      </c>
+      <c r="H152" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I152" t="n">
+        <v>19422</v>
+      </c>
+      <c r="J152" t="n">
+        <v>0</v>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G153" t="n">
+        <v>160</v>
+      </c>
+      <c r="H153" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I153" t="n">
+        <v>17284</v>
+      </c>
+      <c r="J153" t="n">
+        <v>0</v>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G154" t="n">
+        <v>155</v>
+      </c>
+      <c r="H154" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" t="n">
+        <v>16665</v>
+      </c>
+      <c r="J154" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Advanced Micro Devices</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>154.72</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G155" t="n">
+        <v>150</v>
+      </c>
+      <c r="H155" t="n">
+        <v>0</v>
+      </c>
+      <c r="I155" t="n">
+        <v>15416</v>
+      </c>
+      <c r="J155" t="n">
+        <v>0</v>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="156"/>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G157" t="n">
+        <v>155</v>
+      </c>
+      <c r="H157" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I157" t="n">
+        <v>32736</v>
+      </c>
+      <c r="J157" t="n">
+        <v>0</v>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G158" t="n">
+        <v>150</v>
+      </c>
+      <c r="H158" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="I158" t="n">
+        <v>19300</v>
+      </c>
+      <c r="J158" t="n">
+        <v>0</v>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G159" t="n">
+        <v>140</v>
+      </c>
+      <c r="H159" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I159" t="n">
+        <v>18621</v>
+      </c>
+      <c r="J159" t="n">
+        <v>0</v>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G160" t="n">
+        <v>145</v>
+      </c>
+      <c r="H160" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I160" t="n">
+        <v>15556</v>
+      </c>
+      <c r="J160" t="n">
+        <v>0</v>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G161" t="n">
+        <v>160</v>
+      </c>
+      <c r="H161" t="n">
+        <v>25</v>
+      </c>
+      <c r="I161" t="n">
+        <v>15398</v>
+      </c>
+      <c r="J161" t="n">
+        <v>0</v>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G162" t="n">
+        <v>152.5</v>
+      </c>
+      <c r="H162" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I162" t="n">
+        <v>12918</v>
+      </c>
+      <c r="J162" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G163" t="n">
+        <v>148</v>
+      </c>
+      <c r="H163" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I163" t="n">
+        <v>10709</v>
+      </c>
+      <c r="J163" t="n">
+        <v>0</v>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G164" t="n">
+        <v>150</v>
+      </c>
+      <c r="H164" t="n">
+        <v>0</v>
+      </c>
+      <c r="I164" t="n">
+        <v>10129</v>
+      </c>
+      <c r="J164" t="n">
+        <v>0</v>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G165" t="n">
+        <v>149</v>
+      </c>
+      <c r="H165" t="n">
+        <v>0</v>
+      </c>
+      <c r="I165" t="n">
+        <v>8991</v>
+      </c>
+      <c r="J165" t="n">
+        <v>0</v>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Palantir Technologies</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>149.07</v>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G166" t="n">
+        <v>145</v>
+      </c>
+      <c r="H166" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" t="n">
+        <v>8981</v>
+      </c>
+      <c r="J166" t="n">
+        <v>0</v>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="167"/>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G168" t="n">
+        <v>430</v>
+      </c>
+      <c r="H168" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I168" t="n">
+        <v>16599</v>
+      </c>
+      <c r="J168" t="n">
+        <v>0</v>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G169" t="n">
+        <v>440</v>
+      </c>
+      <c r="H169" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I169" t="n">
+        <v>16249</v>
+      </c>
+      <c r="J169" t="n">
+        <v>0</v>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G170" t="n">
+        <v>467.5</v>
+      </c>
+      <c r="H170" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I170" t="n">
+        <v>15565</v>
+      </c>
+      <c r="J170" t="n">
+        <v>0</v>
+      </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G171" t="n">
+        <v>450</v>
+      </c>
+      <c r="H171" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I171" t="n">
+        <v>14740</v>
+      </c>
+      <c r="J171" t="n">
+        <v>0</v>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G172" t="n">
+        <v>420</v>
+      </c>
+      <c r="H172" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I172" t="n">
+        <v>13395</v>
+      </c>
+      <c r="J172" t="n">
+        <v>0</v>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G173" t="n">
+        <v>400</v>
+      </c>
+      <c r="H173" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I173" t="n">
+        <v>8771</v>
+      </c>
+      <c r="J173" t="n">
+        <v>0</v>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G174" t="n">
+        <v>440</v>
+      </c>
+      <c r="H174" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I174" t="n">
+        <v>7524</v>
+      </c>
+      <c r="J174" t="n">
+        <v>0</v>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G175" t="n">
+        <v>465</v>
+      </c>
+      <c r="H175" t="n">
+        <v>25</v>
+      </c>
+      <c r="I175" t="n">
+        <v>6229</v>
+      </c>
+      <c r="J175" t="n">
+        <v>0</v>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G176" t="n">
+        <v>435</v>
+      </c>
+      <c r="H176" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I176" t="n">
+        <v>6214</v>
+      </c>
+      <c r="J176" t="n">
+        <v>0</v>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>MicroStrategy</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>426.4</v>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G177" t="n">
+        <v>425</v>
+      </c>
+      <c r="H177" t="n">
+        <v>0</v>
+      </c>
+      <c r="I177" t="n">
+        <v>6108</v>
+      </c>
+      <c r="J177" t="n">
+        <v>0</v>
+      </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="178"/>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G179" t="n">
+        <v>230</v>
+      </c>
+      <c r="H179" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I179" t="n">
+        <v>49283</v>
+      </c>
+      <c r="J179" t="n">
+        <v>0</v>
+      </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G180" t="n">
+        <v>227.5</v>
+      </c>
+      <c r="H180" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I180" t="n">
+        <v>34711</v>
+      </c>
+      <c r="J180" t="n">
+        <v>0</v>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G181" t="n">
+        <v>232.5</v>
+      </c>
+      <c r="H181" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I181" t="n">
+        <v>19962</v>
+      </c>
+      <c r="J181" t="n">
+        <v>0</v>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G182" t="n">
+        <v>235</v>
+      </c>
+      <c r="H182" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I182" t="n">
+        <v>18787</v>
+      </c>
+      <c r="J182" t="n">
+        <v>0</v>
+      </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G183" t="n">
+        <v>225</v>
+      </c>
+      <c r="H183" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I183" t="n">
+        <v>14454</v>
+      </c>
+      <c r="J183" t="n">
+        <v>0</v>
+      </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G184" t="n">
+        <v>220</v>
+      </c>
+      <c r="H184" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I184" t="n">
+        <v>10990</v>
+      </c>
+      <c r="J184" t="n">
+        <v>0</v>
+      </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G185" t="n">
+        <v>227.5</v>
+      </c>
+      <c r="H185" t="n">
+        <v>0</v>
+      </c>
+      <c r="I185" t="n">
+        <v>10352</v>
+      </c>
+      <c r="J185" t="n">
+        <v>0</v>
+      </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G186" t="n">
+        <v>240</v>
+      </c>
+      <c r="H186" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I186" t="n">
+        <v>9828</v>
+      </c>
+      <c r="J186" t="n">
+        <v>0</v>
+      </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G187" t="n">
+        <v>222.5</v>
+      </c>
+      <c r="H187" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I187" t="n">
+        <v>6615</v>
+      </c>
+      <c r="J187" t="n">
+        <v>0</v>
+      </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>227.47</v>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G188" t="n">
+        <v>260</v>
+      </c>
+      <c r="H188" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I188" t="n">
+        <v>5868</v>
+      </c>
+      <c r="J188" t="n">
+        <v>0</v>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="189"/>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G190" t="n">
+        <v>52</v>
+      </c>
+      <c r="H190" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I190" t="n">
+        <v>22535</v>
+      </c>
+      <c r="J190" t="n">
+        <v>0</v>
+      </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G191" t="n">
+        <v>55</v>
+      </c>
+      <c r="H191" t="n">
+        <v>25</v>
+      </c>
+      <c r="I191" t="n">
+        <v>15957</v>
+      </c>
+      <c r="J191" t="n">
+        <v>0</v>
+      </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G192" t="n">
+        <v>58</v>
+      </c>
+      <c r="H192" t="n">
+        <v>50</v>
+      </c>
+      <c r="I192" t="n">
+        <v>14336</v>
+      </c>
+      <c r="J192" t="n">
+        <v>0</v>
+      </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G193" t="n">
+        <v>50</v>
+      </c>
+      <c r="H193" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="I193" t="n">
+        <v>11672</v>
+      </c>
+      <c r="J193" t="n">
+        <v>0</v>
+      </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G194" t="n">
+        <v>56</v>
+      </c>
+      <c r="H194" t="n">
+        <v>25</v>
+      </c>
+      <c r="I194" t="n">
+        <v>9777</v>
+      </c>
+      <c r="J194" t="n">
+        <v>0</v>
+      </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G195" t="n">
+        <v>53</v>
+      </c>
+      <c r="H195" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I195" t="n">
+        <v>8406</v>
+      </c>
+      <c r="J195" t="n">
+        <v>0</v>
+      </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G196" t="n">
+        <v>46</v>
+      </c>
+      <c r="H196" t="n">
+        <v>25</v>
+      </c>
+      <c r="I196" t="n">
+        <v>7625</v>
+      </c>
+      <c r="J196" t="n">
+        <v>0</v>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G197" t="n">
+        <v>47</v>
+      </c>
+      <c r="H197" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I197" t="n">
+        <v>7249</v>
+      </c>
+      <c r="J197" t="n">
+        <v>0</v>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G198" t="n">
+        <v>51</v>
+      </c>
+      <c r="H198" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I198" t="n">
+        <v>6513</v>
+      </c>
+      <c r="J198" t="n">
+        <v>0</v>
+      </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Supermicro</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>49.86</v>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G199" t="n">
+        <v>50</v>
+      </c>
+      <c r="H199" t="n">
+        <v>0</v>
+      </c>
+      <c r="I199" t="n">
+        <v>5263</v>
+      </c>
+      <c r="J199" t="n">
+        <v>0</v>
+      </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="200"/>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G201" t="n">
+        <v>190</v>
+      </c>
+      <c r="H201" t="n">
+        <v>0</v>
+      </c>
+      <c r="I201" t="n">
+        <v>16604</v>
+      </c>
+      <c r="J201" t="n">
+        <v>0</v>
+      </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G202" t="n">
+        <v>200</v>
+      </c>
+      <c r="H202" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I202" t="n">
+        <v>15764</v>
+      </c>
+      <c r="J202" t="n">
+        <v>0</v>
+      </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G203" t="n">
+        <v>195</v>
+      </c>
+      <c r="H203" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I203" t="n">
+        <v>11038</v>
+      </c>
+      <c r="J203" t="n">
+        <v>0</v>
+      </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E204" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G204" t="n">
+        <v>210</v>
+      </c>
+      <c r="H204" t="n">
+        <v>25</v>
+      </c>
+      <c r="I204" t="n">
+        <v>9862</v>
+      </c>
+      <c r="J204" t="n">
+        <v>0</v>
+      </c>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G205" t="n">
+        <v>205</v>
+      </c>
+      <c r="H205" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I205" t="n">
+        <v>9035</v>
+      </c>
+      <c r="J205" t="n">
+        <v>0</v>
+      </c>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E206" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G206" t="n">
+        <v>192.5</v>
+      </c>
+      <c r="H206" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="I206" t="n">
+        <v>5430</v>
+      </c>
+      <c r="J206" t="n">
+        <v>0</v>
+      </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E207" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G207" t="n">
+        <v>185</v>
+      </c>
+      <c r="H207" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I207" t="n">
+        <v>5317</v>
+      </c>
+      <c r="J207" t="n">
+        <v>0</v>
+      </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E208" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G208" t="n">
+        <v>197.5</v>
+      </c>
+      <c r="H208" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I208" t="n">
+        <v>5236</v>
+      </c>
+      <c r="J208" t="n">
+        <v>0</v>
+      </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E209" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G209" t="n">
+        <v>180</v>
+      </c>
+      <c r="H209" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I209" t="n">
+        <v>5183</v>
+      </c>
+      <c r="J209" t="n">
+        <v>0</v>
+      </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Alphabet Inc. (Class A)</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>191.34</v>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G210" t="n">
+        <v>175</v>
+      </c>
+      <c r="H210" t="n">
+        <v>25</v>
+      </c>
+      <c r="I210" t="n">
+        <v>4821</v>
+      </c>
+      <c r="J210" t="n">
+        <v>0</v>
+      </c>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="211"/>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G212" t="n">
+        <v>720</v>
+      </c>
+      <c r="H212" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I212" t="n">
+        <v>12755</v>
+      </c>
+      <c r="J212" t="n">
+        <v>0</v>
+      </c>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G213" t="n">
+        <v>715</v>
+      </c>
+      <c r="H213" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="I213" t="n">
+        <v>9423</v>
+      </c>
+      <c r="J213" t="n">
+        <v>0</v>
+      </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E214" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G214" t="n">
+        <v>705</v>
+      </c>
+      <c r="H214" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I214" t="n">
+        <v>9318</v>
+      </c>
+      <c r="J214" t="n">
+        <v>0</v>
+      </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G215" t="n">
+        <v>700</v>
+      </c>
+      <c r="H215" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="I215" t="n">
+        <v>9070</v>
+      </c>
+      <c r="J215" t="n">
+        <v>0</v>
+      </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G216" t="n">
+        <v>735</v>
+      </c>
+      <c r="H216" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I216" t="n">
+        <v>8617</v>
+      </c>
+      <c r="J216" t="n">
+        <v>0</v>
+      </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E217" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G217" t="n">
+        <v>710</v>
+      </c>
+      <c r="H217" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="I217" t="n">
+        <v>8491</v>
+      </c>
+      <c r="J217" t="n">
+        <v>0</v>
+      </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E218" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G218" t="n">
+        <v>750</v>
+      </c>
+      <c r="H218" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="I218" t="n">
+        <v>7897</v>
+      </c>
+      <c r="J218" t="n">
+        <v>0</v>
+      </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E219" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G219" t="n">
+        <v>725</v>
+      </c>
+      <c r="H219" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I219" t="n">
+        <v>6875</v>
+      </c>
+      <c r="J219" t="n">
+        <v>0</v>
+      </c>
+      <c r="K219" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>Call</t>
+        </is>
+      </c>
+      <c r="G220" t="n">
+        <v>730</v>
+      </c>
+      <c r="H220" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I220" t="n">
+        <v>6307</v>
+      </c>
+      <c r="J220" t="n">
+        <v>0</v>
+      </c>
+      <c r="K220" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2025-07-23</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>00:56</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Meta Platforms</t>
+        </is>
+      </c>
+      <c r="E221" t="n">
+        <v>704.8099999999999</v>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>Put</t>
+        </is>
+      </c>
+      <c r="G221" t="n">
+        <v>705</v>
+      </c>
+      <c r="H221" t="n">
+        <v>0</v>
+      </c>
+      <c r="I221" t="n">
+        <v>5638</v>
+      </c>
+      <c r="J221" t="n">
+        <v>0</v>
+      </c>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>2025-07-25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>